<commit_message>
Major system update: Import Excel data, fix ingredient prices, add order statuses, increase quantities x10
</commit_message>
<xml_diff>
--- a/ingredients.xlsx
+++ b/ingredients.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,15 +466,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Нори</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
+        <v>10000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="3">
@@ -483,11 +487,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>банан</t>
+          <t>Рис</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -495,7 +499,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="4">
@@ -504,11 +508,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>васаби</t>
+          <t>банан</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -516,7 +520,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="5">
@@ -525,11 +529,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>вода</t>
+          <t>васаби</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -537,7 +541,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
@@ -546,11 +550,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>икра масаго</t>
+          <t>вода</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -567,11 +571,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>имбирь</t>
+          <t>икра масага</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -579,7 +583,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="8">
@@ -588,11 +592,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>кап семка</t>
+          <t>имбир</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -600,7 +604,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="9">
@@ -609,11 +613,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>киви</t>
+          <t>имбирь</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -621,7 +625,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="10">
@@ -630,11 +634,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>клубника</t>
+          <t>кап семка</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -642,7 +646,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="11">
@@ -651,11 +655,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>кляр</t>
+          <t>капч лосось</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -663,7 +667,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="12">
@@ -672,11 +676,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>краб</t>
+          <t>капчен кур</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -684,7 +688,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="13">
@@ -693,11 +697,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>кунжут</t>
+          <t>киви</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,7 +709,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14">
@@ -714,11 +718,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>курица</t>
+          <t>клубника</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -726,7 +730,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15">
@@ -735,11 +739,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>листья салата</t>
+          <t>кляр</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -747,7 +751,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="16">
@@ -756,11 +760,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>лосось</t>
+          <t>краб</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -768,7 +772,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="17">
@@ -777,11 +781,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>майонез</t>
+          <t>кунжут</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -789,7 +793,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18">
@@ -798,15 +802,19 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>мицукан</t>
+          <t>курица</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="inlineStr"/>
+        <v>10000</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="19">
@@ -815,11 +823,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>мука</t>
+          <t>листья салата</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -827,7 +835,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="20">
@@ -836,19 +844,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>нори</t>
+          <t>лосось</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>шт</t>
+          <t>г</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -857,11 +865,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>огурец</t>
+          <t>майонез</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -869,7 +877,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="22">
@@ -878,11 +886,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>омлет</t>
+          <t>масага кр</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -890,7 +898,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="23">
@@ -899,11 +907,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>остр соус</t>
+          <t>мицукан</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -911,7 +919,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="24">
@@ -920,11 +928,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>перец</t>
+          <t>мука</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -932,7 +940,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="25">
@@ -941,11 +949,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>помидор</t>
+          <t>нори</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -953,7 +961,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="26">
@@ -962,11 +970,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>рис</t>
+          <t>огурец</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -974,7 +982,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="27">
@@ -983,15 +991,19 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>сахар</t>
+          <t>огурцы</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" t="inlineStr"/>
+        <v>10000</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="28">
@@ -1000,11 +1012,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>семга</t>
+          <t>омлет</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1012,7 +1024,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="29">
@@ -1021,11 +1033,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>соевый соус</t>
+          <t>остр соус</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1033,7 +1045,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="30">
@@ -1042,11 +1054,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>соль</t>
+          <t>перец</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1054,7 +1066,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="31">
@@ -1063,19 +1075,19 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>сприн тесто</t>
+          <t>помидор</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>шт</t>
+          <t>г</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="32">
@@ -1084,11 +1096,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>сухари</t>
+          <t>рис</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1096,7 +1108,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="33">
@@ -1105,11 +1117,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>сыр пармезан</t>
+          <t>сахар</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1117,7 +1129,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="34">
@@ -1126,11 +1138,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>сыр соус</t>
+          <t>семга</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1138,7 +1150,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="35">
@@ -1147,11 +1159,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>сыр творожный</t>
+          <t>соевый соус</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1159,7 +1171,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="36">
@@ -1168,11 +1180,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>сыр чеддер</t>
+          <t>соль</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1180,7 +1192,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="37">
@@ -1189,11 +1201,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>сырный соус</t>
+          <t>сприн тесто</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1201,7 +1213,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38">
@@ -1210,11 +1222,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>угорь</t>
+          <t>сухари</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1222,7 +1234,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="39">
@@ -1231,11 +1243,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>унаги соус</t>
+          <t>сыр пармизан</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1243,7 +1255,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="40">
@@ -1252,11 +1264,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>чипсы</t>
+          <t>сыр соус</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1264,7 +1276,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="41">
@@ -1273,11 +1285,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ширачи</t>
+          <t>сыр твор</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1285,7 +1297,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="42">
@@ -1294,11 +1306,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>шоколад</t>
+          <t>сыр творож</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1306,7 +1318,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="43">
@@ -1315,11 +1327,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>яблоко</t>
+          <t>сыр товр</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1327,7 +1339,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="44">
@@ -1336,19 +1348,229 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>сыр чеддер</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>сырный соус</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>сырный соус 350</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>твор сыр</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>угорь</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>унаги соус</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>чипсы</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ширачи</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>шоколад</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>яблоко</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>яйцо</t>
         </is>
       </c>
-      <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>шт</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>0</v>
+      <c r="C54" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>г</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>0.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>